<commit_message>
Update javascript for page
</commit_message>
<xml_diff>
--- a/Documents/SprintBacklog.xlsx
+++ b/Documents/SprintBacklog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Desktop/Capstone/CTSProject/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="41">
   <si>
     <t>Status</t>
   </si>
@@ -138,6 +138,15 @@
   </si>
   <si>
     <t>- Proposed solution</t>
+  </si>
+  <si>
+    <t>Implement prototype</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>- Manage user</t>
   </si>
 </sst>
 </file>
@@ -241,7 +250,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -271,8 +280,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -552,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="111" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -816,7 +824,7 @@
       <c r="E18" s="6"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="13" t="s">
         <v>35</v>
       </c>
       <c r="B19" s="6"/>
@@ -825,7 +833,7 @@
       <c r="E19" s="6"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="13" t="s">
         <v>36</v>
       </c>
       <c r="B20" s="6"/>
@@ -834,7 +842,7 @@
       <c r="E20" s="6"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="13" t="s">
         <v>37</v>
       </c>
       <c r="B21" s="6"/>
@@ -843,13 +851,14 @@
       <c r="E21" s="6"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="13"/>
+      <c r="A22" s="9"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
@@ -878,88 +887,155 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="8"/>
+      <c r="A26" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
-      <c r="E26" s="6">
-        <v>3</v>
-      </c>
+      <c r="E26" s="6"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="8" t="s">
-        <v>6</v>
+      <c r="A27" s="13" t="s">
+        <v>27</v>
       </c>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
-      <c r="E27" s="6">
-        <v>2</v>
-      </c>
+      <c r="E27" s="6"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="8" t="s">
-        <v>6</v>
+      <c r="A28" s="13" t="s">
+        <v>40</v>
       </c>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
-      <c r="E28" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B29" s="4">
-        <v>5</v>
-      </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="13"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="A30" s="13"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
-      <c r="E30" s="6">
-        <v>8</v>
-      </c>
+      <c r="E30" s="6"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="8" t="s">
-        <v>6</v>
-      </c>
+      <c r="A31" s="13"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
-      <c r="E31" s="6">
-        <v>3</v>
-      </c>
+      <c r="E31" s="6"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="8" t="s">
-        <v>6</v>
-      </c>
+      <c r="A32" s="13"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
-      <c r="E32" s="6">
-        <v>1.5</v>
-      </c>
+      <c r="E32" s="6"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="A33" s="13"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
-      <c r="E33" s="6">
+      <c r="E33" s="6"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="13"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="9"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38" s="4">
+        <v>5</v>
+      </c>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Complete plan overview page
</commit_message>
<xml_diff>
--- a/Documents/SprintBacklog.xlsx
+++ b/Documents/SprintBacklog.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1160" windowWidth="24960" windowHeight="14100" tabRatio="500"/>
+    <workbookView xWindow="420" yWindow="600" windowWidth="24960" windowHeight="14100" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint Backlog" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="64">
   <si>
     <t>Status</t>
   </si>
@@ -44,12 +44,6 @@
     <t>Responsible</t>
   </si>
   <si>
-    <t xml:space="preserve">Task </t>
-  </si>
-  <si>
-    <t>Task</t>
-  </si>
-  <si>
     <t>Item</t>
   </si>
   <si>
@@ -119,9 +113,6 @@
     <t>NguyenVT</t>
   </si>
   <si>
-    <t>1.5 day</t>
-  </si>
-  <si>
     <t>0.5 day</t>
   </si>
   <si>
@@ -140,20 +131,129 @@
     <t>- Proposed solution</t>
   </si>
   <si>
-    <t>Implement prototype</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>- Manage user</t>
+    <t>In process</t>
+  </si>
+  <si>
+    <t>- Functional requirement, role responsibility</t>
+  </si>
+  <si>
+    <t>2 days</t>
+  </si>
+  <si>
+    <t>Nguyen VT</t>
+  </si>
+  <si>
+    <t>3 days</t>
+  </si>
+  <si>
+    <t>- Master page</t>
+  </si>
+  <si>
+    <t>- Learner page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    + Manage user page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    + Manage brand page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    + Manage course page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    + Manage skill page</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+ Problem definition</t>
+    </r>
+  </si>
+  <si>
+    <t>Report 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    + Project Organization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    + Project Management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    + Coding convention</t>
+  </si>
+  <si>
+    <t>- Manage page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Manage Page </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   + </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   + Finish manage course page</t>
+  </si>
+  <si>
+    <t>To do</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   + Manage plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   + Learning page (Quiz)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   + Learning page (Text / powerpoint / video)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   + View quiz result page </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+ Plan overview page</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">    + User plan page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement prototype  </t>
+  </si>
+  <si>
+    <t>1 days</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -221,7 +321,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -244,22 +344,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -268,19 +377,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -560,484 +669,710 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="111" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="46.83203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="1"/>
-    <col min="5" max="5" width="19.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="13" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6" t="s">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6" t="s">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6" t="s">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="13" t="s">
-        <v>35</v>
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
+        <v>32</v>
       </c>
       <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="13" t="s">
+      <c r="C19" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="9"/>
       <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-    </row>
-    <row r="24" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
+      <c r="C22" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="B25" s="6"/>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="13" t="s">
-        <v>27</v>
+      <c r="A27" s="12" t="s">
+        <v>25</v>
       </c>
       <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
+      <c r="C27" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B28" s="6"/>
+      <c r="A28" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="8"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="13"/>
+      <c r="A29" s="12" t="s">
+        <v>42</v>
+      </c>
       <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
+      <c r="C29" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="13"/>
+      <c r="A30" s="12" t="s">
+        <v>43</v>
+      </c>
       <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
+      <c r="C30" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="13"/>
+      <c r="A31" s="12" t="s">
+        <v>44</v>
+      </c>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="13"/>
+      <c r="A32" s="12" t="s">
+        <v>45</v>
+      </c>
       <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
+      <c r="C32" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="13"/>
+      <c r="A33" s="9" t="s">
+        <v>41</v>
+      </c>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="13"/>
+      <c r="A34" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
+      <c r="C34" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="9"/>
+      <c r="A35" s="9" t="s">
+        <v>60</v>
+      </c>
       <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
+      <c r="C35" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="8" t="s">
-        <v>39</v>
+      <c r="A36" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
-      <c r="E36" s="6">
-        <v>2</v>
-      </c>
+      <c r="E36" s="6"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="8" t="s">
-        <v>39</v>
+      <c r="A37" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B38" s="4">
-        <v>5</v>
-      </c>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
+      <c r="C37" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6">
-        <v>8</v>
+      <c r="C39" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="8" t="s">
-        <v>6</v>
+      <c r="A40" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6">
-        <v>1.5</v>
-      </c>
+      <c r="C40" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B41" s="4"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="8" t="s">
-        <v>7</v>
+      <c r="A42" s="9" t="s">
+        <v>62</v>
       </c>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
-      <c r="E42" s="6">
-        <v>2</v>
-      </c>
+      <c r="E42" s="6"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="8"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B50" s="6"/>
+      <c r="C50" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B51" s="6"/>
+      <c r="C51" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="8"/>
+      <c r="B52" s="6"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="8"/>
+      <c r="B53" s="6"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" s="8"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
[Issue #12] Incomplete class diagram
</commit_message>
<xml_diff>
--- a/Documents/SprintBacklog.xlsx
+++ b/Documents/SprintBacklog.xlsx
@@ -9,10 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="420" yWindow="600" windowWidth="24960" windowHeight="14100" tabRatio="500"/>
+    <workbookView xWindow="420" yWindow="600" windowWidth="24960" windowHeight="14100" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint Backlog" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint 1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sprint 2" sheetId="3" r:id="rId3"/>
+    <sheet name="Sprint 3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="100">
   <si>
     <t>Status</t>
   </si>
@@ -301,12 +304,60 @@
   <si>
     <t>Class diagram</t>
   </si>
+  <si>
+    <t>Backlog Item</t>
+  </si>
+  <si>
+    <t>Original Estimate</t>
+  </si>
+  <si>
+    <t>Day 1</t>
+  </si>
+  <si>
+    <t>Day 2</t>
+  </si>
+  <si>
+    <t>Day 3</t>
+  </si>
+  <si>
+    <t>Day 4</t>
+  </si>
+  <si>
+    <t>Day 5</t>
+  </si>
+  <si>
+    <t>Sprint Review</t>
+  </si>
+  <si>
+    <t>User Story #1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task </t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>User Story #2</t>
+  </si>
+  <si>
+    <t>User Story #3</t>
+  </si>
+  <si>
+    <t>User Story #4</t>
+  </si>
+  <si>
+    <t>User Story #5</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -353,8 +404,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -373,8 +438,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC9C9C9"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEDEDED"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBFBFBF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -417,15 +506,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -453,18 +581,54 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -742,7 +906,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="111" workbookViewId="0">
+    <sheetView zoomScale="111" workbookViewId="0">
       <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
@@ -756,13 +920,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="A1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -1348,7 +1512,7 @@
       <c r="E44" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F44" s="14" t="s">
+      <c r="F44" s="13" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1366,7 +1530,7 @@
       <c r="E45" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F45" s="14" t="s">
+      <c r="F45" s="13" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1607,4 +1771,1496 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="6">
+        <v>7</v>
+      </c>
+      <c r="F3" s="6">
+        <v>5</v>
+      </c>
+      <c r="G3" s="6">
+        <v>3</v>
+      </c>
+      <c r="H3" s="6">
+        <v>0</v>
+      </c>
+      <c r="I3" s="6">
+        <v>0</v>
+      </c>
+      <c r="J3" s="6">
+        <v>0</v>
+      </c>
+      <c r="K3" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="6">
+        <v>3</v>
+      </c>
+      <c r="F4" s="6">
+        <v>1</v>
+      </c>
+      <c r="G4" s="6">
+        <v>1</v>
+      </c>
+      <c r="H4" s="6">
+        <v>5</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0</v>
+      </c>
+      <c r="J4" s="6">
+        <v>1</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="6">
+        <v>1</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0</v>
+      </c>
+      <c r="H5" s="6">
+        <v>3</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0</v>
+      </c>
+      <c r="J5" s="6">
+        <v>0</v>
+      </c>
+      <c r="K5" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F6" s="6">
+        <v>1</v>
+      </c>
+      <c r="G6" s="6">
+        <v>2</v>
+      </c>
+      <c r="H6" s="6">
+        <v>3</v>
+      </c>
+      <c r="I6" s="6">
+        <v>1</v>
+      </c>
+      <c r="J6" s="6">
+        <v>0</v>
+      </c>
+      <c r="K6" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="6">
+        <v>3</v>
+      </c>
+      <c r="F8" s="6">
+        <v>3</v>
+      </c>
+      <c r="G8" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="H8" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="I8" s="6">
+        <v>0</v>
+      </c>
+      <c r="J8" s="6">
+        <v>0</v>
+      </c>
+      <c r="K8" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="6">
+        <v>3</v>
+      </c>
+      <c r="F9" s="6">
+        <v>5</v>
+      </c>
+      <c r="G9" s="6">
+        <v>5</v>
+      </c>
+      <c r="H9" s="6">
+        <v>1</v>
+      </c>
+      <c r="I9" s="6">
+        <v>1</v>
+      </c>
+      <c r="J9" s="6">
+        <v>1</v>
+      </c>
+      <c r="K9" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="6">
+        <v>2</v>
+      </c>
+      <c r="F10" s="6">
+        <v>2</v>
+      </c>
+      <c r="G10" s="6">
+        <v>5</v>
+      </c>
+      <c r="H10" s="6">
+        <v>0</v>
+      </c>
+      <c r="I10" s="6">
+        <v>1</v>
+      </c>
+      <c r="J10" s="6">
+        <v>0</v>
+      </c>
+      <c r="K10" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="6">
+        <v>5</v>
+      </c>
+      <c r="F11" s="6">
+        <v>5</v>
+      </c>
+      <c r="G11" s="6">
+        <v>9</v>
+      </c>
+      <c r="H11" s="6">
+        <v>5</v>
+      </c>
+      <c r="I11" s="6">
+        <v>1</v>
+      </c>
+      <c r="J11" s="6">
+        <v>0</v>
+      </c>
+      <c r="K11" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="6">
+        <v>8</v>
+      </c>
+      <c r="F13" s="6">
+        <v>6</v>
+      </c>
+      <c r="G13" s="6">
+        <v>0</v>
+      </c>
+      <c r="H13" s="6">
+        <v>0</v>
+      </c>
+      <c r="I13" s="6">
+        <v>0</v>
+      </c>
+      <c r="J13" s="6">
+        <v>0</v>
+      </c>
+      <c r="K13" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="6">
+        <v>3</v>
+      </c>
+      <c r="F14" s="6">
+        <v>1</v>
+      </c>
+      <c r="G14" s="6">
+        <v>3</v>
+      </c>
+      <c r="H14" s="6">
+        <v>3</v>
+      </c>
+      <c r="I14" s="6">
+        <v>3</v>
+      </c>
+      <c r="J14" s="6">
+        <v>0</v>
+      </c>
+      <c r="K14" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="F15" s="6">
+        <v>1</v>
+      </c>
+      <c r="G15" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="H15" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="I15" s="6">
+        <v>1</v>
+      </c>
+      <c r="J15" s="6">
+        <v>1</v>
+      </c>
+      <c r="K15" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="6">
+        <v>2</v>
+      </c>
+      <c r="F16" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="G16" s="6">
+        <v>0</v>
+      </c>
+      <c r="H16" s="6">
+        <v>0</v>
+      </c>
+      <c r="I16" s="6">
+        <v>0</v>
+      </c>
+      <c r="J16" s="6">
+        <v>0</v>
+      </c>
+      <c r="K16" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="6">
+        <v>9</v>
+      </c>
+      <c r="F18" s="6">
+        <v>4</v>
+      </c>
+      <c r="G18" s="6">
+        <v>2</v>
+      </c>
+      <c r="H18" s="6">
+        <v>2</v>
+      </c>
+      <c r="I18" s="6">
+        <v>1</v>
+      </c>
+      <c r="J18" s="6">
+        <v>1</v>
+      </c>
+      <c r="K18" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="6">
+        <v>6</v>
+      </c>
+      <c r="F19" s="6">
+        <v>6</v>
+      </c>
+      <c r="G19" s="6">
+        <v>3</v>
+      </c>
+      <c r="H19" s="6">
+        <v>3</v>
+      </c>
+      <c r="I19" s="6">
+        <v>3</v>
+      </c>
+      <c r="J19" s="6">
+        <v>1</v>
+      </c>
+      <c r="K19" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="6">
+        <v>6</v>
+      </c>
+      <c r="F20" s="6">
+        <v>2</v>
+      </c>
+      <c r="G20" s="6">
+        <v>8</v>
+      </c>
+      <c r="H20" s="6">
+        <v>8</v>
+      </c>
+      <c r="I20" s="6">
+        <v>1</v>
+      </c>
+      <c r="J20" s="6">
+        <v>0</v>
+      </c>
+      <c r="K20" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F21" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="G21" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="H21" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="I21" s="6">
+        <v>0</v>
+      </c>
+      <c r="J21" s="6">
+        <v>0</v>
+      </c>
+      <c r="K21" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="6">
+        <v>2</v>
+      </c>
+      <c r="F23" s="6">
+        <v>1</v>
+      </c>
+      <c r="G23" s="6">
+        <v>1</v>
+      </c>
+      <c r="H23" s="6">
+        <v>1</v>
+      </c>
+      <c r="I23" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="J23" s="6">
+        <v>1</v>
+      </c>
+      <c r="K23" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="6">
+        <v>6</v>
+      </c>
+      <c r="F24" s="6">
+        <v>6</v>
+      </c>
+      <c r="G24" s="6">
+        <v>6</v>
+      </c>
+      <c r="H24" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="I24" s="6">
+        <v>3</v>
+      </c>
+      <c r="J24" s="6">
+        <v>9</v>
+      </c>
+      <c r="K24" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="6">
+        <v>9</v>
+      </c>
+      <c r="F25" s="6">
+        <v>9</v>
+      </c>
+      <c r="G25" s="6">
+        <v>9</v>
+      </c>
+      <c r="H25" s="6">
+        <v>4</v>
+      </c>
+      <c r="I25" s="6">
+        <v>3</v>
+      </c>
+      <c r="J25" s="6">
+        <v>3</v>
+      </c>
+      <c r="K25" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F26" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="G26" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="H26" s="6">
+        <v>1</v>
+      </c>
+      <c r="I26" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="J26" s="6">
+        <v>0</v>
+      </c>
+      <c r="K26" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19">
+        <f>SUM(E2:E26)</f>
+        <v>78</v>
+      </c>
+      <c r="F27" s="19">
+        <f>SUM(F3:F26)</f>
+        <v>60</v>
+      </c>
+      <c r="G27" s="19">
+        <f>SUM(G2:G26)</f>
+        <v>59</v>
+      </c>
+      <c r="H27" s="19">
+        <f>SUM(H2:H26)</f>
+        <v>41</v>
+      </c>
+      <c r="I27" s="19">
+        <f>SUM(I2:I26)</f>
+        <v>20</v>
+      </c>
+      <c r="J27" s="19">
+        <f>SUM(J2:J26)</f>
+        <v>18</v>
+      </c>
+      <c r="K27" s="19">
+        <f>SUM(K2:K26)</f>
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="27"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="27">
+        <v>7</v>
+      </c>
+      <c r="F3" s="27">
+        <v>5</v>
+      </c>
+      <c r="G3" s="27">
+        <v>3</v>
+      </c>
+      <c r="H3" s="27">
+        <v>0</v>
+      </c>
+      <c r="I3" s="27">
+        <v>0</v>
+      </c>
+      <c r="J3" s="27">
+        <v>0</v>
+      </c>
+      <c r="K3" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="27"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="27">
+        <v>3</v>
+      </c>
+      <c r="F4" s="27">
+        <v>1</v>
+      </c>
+      <c r="G4" s="27">
+        <v>1</v>
+      </c>
+      <c r="H4" s="27">
+        <v>5</v>
+      </c>
+      <c r="I4" s="27">
+        <v>0</v>
+      </c>
+      <c r="J4" s="27">
+        <v>1</v>
+      </c>
+      <c r="K4" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="27"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="27">
+        <v>1</v>
+      </c>
+      <c r="F5" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="G5" s="27">
+        <v>0</v>
+      </c>
+      <c r="H5" s="27">
+        <v>3</v>
+      </c>
+      <c r="I5" s="27">
+        <v>0</v>
+      </c>
+      <c r="J5" s="27">
+        <v>0</v>
+      </c>
+      <c r="K5" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="27"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="F6" s="27">
+        <v>1</v>
+      </c>
+      <c r="G6" s="27">
+        <v>2</v>
+      </c>
+      <c r="H6" s="27">
+        <v>3</v>
+      </c>
+      <c r="I6" s="27">
+        <v>1</v>
+      </c>
+      <c r="J6" s="27">
+        <v>0</v>
+      </c>
+      <c r="K6" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" s="23"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" s="27"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="27">
+        <v>3</v>
+      </c>
+      <c r="F8" s="27">
+        <v>3</v>
+      </c>
+      <c r="G8" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="H8" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="I8" s="27">
+        <v>0</v>
+      </c>
+      <c r="J8" s="27">
+        <v>0</v>
+      </c>
+      <c r="K8" s="27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" s="27"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="27">
+        <v>3</v>
+      </c>
+      <c r="F9" s="27">
+        <v>5</v>
+      </c>
+      <c r="G9" s="27">
+        <v>5</v>
+      </c>
+      <c r="H9" s="27">
+        <v>1</v>
+      </c>
+      <c r="I9" s="27">
+        <v>1</v>
+      </c>
+      <c r="J9" s="27">
+        <v>1</v>
+      </c>
+      <c r="K9" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="B10" s="27"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="27">
+        <v>2</v>
+      </c>
+      <c r="F10" s="27">
+        <v>2</v>
+      </c>
+      <c r="G10" s="27">
+        <v>5</v>
+      </c>
+      <c r="H10" s="27">
+        <v>0</v>
+      </c>
+      <c r="I10" s="27">
+        <v>1</v>
+      </c>
+      <c r="J10" s="27">
+        <v>0</v>
+      </c>
+      <c r="K10" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" s="27"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="27">
+        <v>5</v>
+      </c>
+      <c r="F11" s="27">
+        <v>5</v>
+      </c>
+      <c r="G11" s="27">
+        <v>9</v>
+      </c>
+      <c r="H11" s="27">
+        <v>5</v>
+      </c>
+      <c r="I11" s="27">
+        <v>1</v>
+      </c>
+      <c r="J11" s="27">
+        <v>0</v>
+      </c>
+      <c r="K11" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A12" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" s="23"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" s="27"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="27">
+        <v>8</v>
+      </c>
+      <c r="F13" s="27">
+        <v>6</v>
+      </c>
+      <c r="G13" s="27">
+        <v>0</v>
+      </c>
+      <c r="H13" s="27">
+        <v>0</v>
+      </c>
+      <c r="I13" s="27">
+        <v>0</v>
+      </c>
+      <c r="J13" s="27">
+        <v>0</v>
+      </c>
+      <c r="K13" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="B14" s="27"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="27">
+        <v>3</v>
+      </c>
+      <c r="F14" s="27">
+        <v>1</v>
+      </c>
+      <c r="G14" s="27">
+        <v>3</v>
+      </c>
+      <c r="H14" s="27">
+        <v>3</v>
+      </c>
+      <c r="I14" s="27">
+        <v>3</v>
+      </c>
+      <c r="J14" s="27">
+        <v>0</v>
+      </c>
+      <c r="K14" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" s="27"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="27">
+        <v>1.5</v>
+      </c>
+      <c r="F15" s="27">
+        <v>1</v>
+      </c>
+      <c r="G15" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="H15" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="I15" s="27">
+        <v>1</v>
+      </c>
+      <c r="J15" s="27">
+        <v>1</v>
+      </c>
+      <c r="K15" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" s="27"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="27">
+        <v>2</v>
+      </c>
+      <c r="F16" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="G16" s="27">
+        <v>0</v>
+      </c>
+      <c r="H16" s="27">
+        <v>0</v>
+      </c>
+      <c r="I16" s="27">
+        <v>0</v>
+      </c>
+      <c r="J16" s="27">
+        <v>0</v>
+      </c>
+      <c r="K16" s="27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A17" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" s="23"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="B18" s="27"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="27">
+        <v>9</v>
+      </c>
+      <c r="F18" s="27">
+        <v>4</v>
+      </c>
+      <c r="G18" s="27">
+        <v>2</v>
+      </c>
+      <c r="H18" s="27">
+        <v>2</v>
+      </c>
+      <c r="I18" s="27">
+        <v>1</v>
+      </c>
+      <c r="J18" s="27">
+        <v>1</v>
+      </c>
+      <c r="K18" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="B19" s="27"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="27">
+        <v>6</v>
+      </c>
+      <c r="F19" s="27">
+        <v>6</v>
+      </c>
+      <c r="G19" s="27">
+        <v>3</v>
+      </c>
+      <c r="H19" s="27">
+        <v>3</v>
+      </c>
+      <c r="I19" s="27">
+        <v>3</v>
+      </c>
+      <c r="J19" s="27">
+        <v>1</v>
+      </c>
+      <c r="K19" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" s="27"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="27">
+        <v>6</v>
+      </c>
+      <c r="F20" s="27">
+        <v>2</v>
+      </c>
+      <c r="G20" s="27">
+        <v>8</v>
+      </c>
+      <c r="H20" s="27">
+        <v>8</v>
+      </c>
+      <c r="I20" s="27">
+        <v>1</v>
+      </c>
+      <c r="J20" s="27">
+        <v>0</v>
+      </c>
+      <c r="K20" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" s="27"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="F21" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="G21" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="H21" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="I21" s="27">
+        <v>0</v>
+      </c>
+      <c r="J21" s="27">
+        <v>0</v>
+      </c>
+      <c r="K21" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A22" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="B22" s="23"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="25"/>
+      <c r="K22" s="25"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23" s="27"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="27">
+        <v>2</v>
+      </c>
+      <c r="F23" s="27">
+        <v>1</v>
+      </c>
+      <c r="G23" s="27">
+        <v>1</v>
+      </c>
+      <c r="H23" s="27">
+        <v>1</v>
+      </c>
+      <c r="I23" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="J23" s="27">
+        <v>1</v>
+      </c>
+      <c r="K23" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" s="27"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="27">
+        <v>6</v>
+      </c>
+      <c r="F24" s="27">
+        <v>6</v>
+      </c>
+      <c r="G24" s="27">
+        <v>6</v>
+      </c>
+      <c r="H24" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="I24" s="27">
+        <v>3</v>
+      </c>
+      <c r="J24" s="27">
+        <v>9</v>
+      </c>
+      <c r="K24" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" s="27"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="27">
+        <v>9</v>
+      </c>
+      <c r="F25" s="27">
+        <v>9</v>
+      </c>
+      <c r="G25" s="27">
+        <v>9</v>
+      </c>
+      <c r="H25" s="27">
+        <v>4</v>
+      </c>
+      <c r="I25" s="27">
+        <v>3</v>
+      </c>
+      <c r="J25" s="27">
+        <v>3</v>
+      </c>
+      <c r="K25" s="27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="B26" s="27"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="F26" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="G26" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="H26" s="27">
+        <v>1</v>
+      </c>
+      <c r="I26" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="J26" s="27">
+        <v>0</v>
+      </c>
+      <c r="K26" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" s="30"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30">
+        <v>78</v>
+      </c>
+      <c r="F27" s="30">
+        <v>60</v>
+      </c>
+      <c r="G27" s="30">
+        <v>59</v>
+      </c>
+      <c r="H27" s="30">
+        <v>41</v>
+      </c>
+      <c r="I27" s="30">
+        <v>20</v>
+      </c>
+      <c r="J27" s="30">
+        <v>18</v>
+      </c>
+      <c r="K27" s="30">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>